<commit_message>
2 nd commit 4/28
</commit_message>
<xml_diff>
--- a/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
+++ b/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\git\Team23-LMS-Hackathon\LMS_Hackathon\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CFAD8DF-AC1B-4704-B88D-7734645A8A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2236A-C912-4B78-A0D5-0542C3169736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,10 +44,10 @@
     <t>programDescription</t>
   </si>
   <si>
-    <t>Team23JavaSelinium</t>
-  </si>
-  <si>
-    <t>AutomationTeam23coding</t>
+    <t>Team23JavaS</t>
+  </si>
+  <si>
+    <t>AutomationTeam23cod</t>
   </si>
 </sst>
 </file>
@@ -373,7 +373,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add User Scenario is committed
</commit_message>
<xml_diff>
--- a/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
+++ b/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
@@ -3,25 +3,22 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\git\Team23-LMS-Hackathon\LMS_Hackathon\src\test\resources\Test_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4C2236A-C912-4B78-A0D5-0542C3169736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{BE1CA641-F99C-4776-A092-8B14C76CFDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="ProgramModule" sheetId="2" r:id="rId2"/>
+    <sheet name="AddUser" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1:I6"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="55">
   <si>
     <t>username</t>
   </si>
@@ -48,13 +45,151 @@
   </si>
   <si>
     <t>AutomationTeam23cod</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>MiddleName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>PhoneNum</t>
+  </si>
+  <si>
+    <t>LinkedUrl</t>
+  </si>
+  <si>
+    <t>UserRole</t>
+  </si>
+  <si>
+    <t>RoleStatus</t>
+  </si>
+  <si>
+    <t>VisaStatus</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>UnderGrad</t>
+  </si>
+  <si>
+    <t>PostGrad</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>UserComments</t>
+  </si>
+  <si>
+    <t>Rachael</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t>Irving</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>H4-EAD</t>
+  </si>
+  <si>
+    <t>Mony</t>
+  </si>
+  <si>
+    <t>www.linkedin.com</t>
+  </si>
+  <si>
+    <t>sde12@gmail.com</t>
+  </si>
+  <si>
+    <t>UG</t>
+  </si>
+  <si>
+    <t>PG</t>
+  </si>
+  <si>
+    <t>EST</t>
+  </si>
+  <si>
+    <t>User is created</t>
+  </si>
+  <si>
+    <t>J</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>123-Irving</t>
+  </si>
+  <si>
+    <t>www.linkedurl.com</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>IndianTime</t>
+  </si>
+  <si>
+    <t>Raymond</t>
+  </si>
+  <si>
+    <t>Vinoth</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>R01</t>
+  </si>
+  <si>
+    <t>hjy@gmail.com</t>
+  </si>
+  <si>
+    <t>CST</t>
+  </si>
+  <si>
+    <t>New User is Created</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Bony</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>ghe@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -65,7 +200,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -73,7 +207,8 @@
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
@@ -81,7 +216,12 @@
       <sz val="10"/>
       <color rgb="FF2A00FF"/>
       <name val="Consolas"/>
-      <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,11 +244,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -329,16 +471,15 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="22.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -346,7 +487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -354,8 +495,8 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -363,42 +504,280 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0BF687-F25D-4899-BC43-1B7EA74765DC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:N7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="14" max="14" width="14.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3">
+        <v>5678905432</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B3" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="3">
+        <v>78654</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="3">
+        <v>123</v>
+      </c>
+      <c r="L4" s="3">
+        <v>345</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="3">
+        <v>3452678910</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="3">
+        <v>3456789045</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F7" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
committing BatchPage stepdefinition and feature files
</commit_message>
<xml_diff>
--- a/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
+++ b/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yours\git\Team23-LMS-Hackathon\LMS_Hackathon\src\test\resources\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amaniknadan/IdeaProjects/Team23-LMS-Hackathon/LMS_Hackathon/src/test/resources/Test_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ADC43A-10E9-466D-86FE-C9E9BBA5E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED40F211-67E2-254B-A9D1-7748685AB6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="39600" windowHeight="25100" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>username</t>
   </si>
@@ -67,15 +67,9 @@
     <t>noc</t>
   </si>
   <si>
-    <t>Batch23</t>
-  </si>
-  <si>
     <t>Batch Description</t>
   </si>
   <si>
-    <t>amazon</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -212,6 +206,24 @@
   </si>
   <si>
     <t>ghe@gmail.com</t>
+  </si>
+  <si>
+    <t>AWS1</t>
+  </si>
+  <si>
+    <t>Batch23-1</t>
+  </si>
+  <si>
+    <t>Batch24-1</t>
+  </si>
+  <si>
+    <t>Batch25-1</t>
+  </si>
+  <si>
+    <t>$@#$23&amp;&amp;&amp;</t>
+  </si>
+  <si>
+    <t>dats</t>
   </si>
 </sst>
 </file>
@@ -229,16 +241,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -265,6 +280,7 @@
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -287,15 +303,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -521,12 +535,12 @@
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="24.7109375" customWidth="1"/>
+    <col min="1" max="2" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="12.75">
+    <row r="1" spans="1:2" ht="13">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -534,7 +548,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="12.75">
+    <row r="2" spans="1:2" ht="13">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -564,13 +578,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="14">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -595,240 +609,224 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F22F8EA-D627-4EC3-9A1D-2EB34ED5611E}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="7" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="1">
+        <v>5678905432</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="7">
-        <v>5678905432</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8" t="s">
+      <c r="K3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="1">
+        <v>78654</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="7">
-        <v>78654</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="K4" s="1">
+        <v>123</v>
+      </c>
+      <c r="L4" s="1">
+        <v>345</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7" t="s">
+      <c r="N4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="7">
-        <v>123</v>
-      </c>
-      <c r="L4" s="7">
-        <v>345</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="7" t="s">
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="1">
+        <v>3452678910</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="7">
-        <v>3452678910</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="K5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="L5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="N5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3456789045</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3456789045</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -844,15 +842,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCADA34F-E7EC-194B-A56A-7E273D062B57}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="13.5">
+    <row r="1" spans="1:5">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -871,19 +872,70 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="5" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
       </c>
       <c r="E2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5">
+        <v>123</v>
+      </c>
+      <c r="D5">
+        <v>23</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2nd Committ on 5/1/2024
</commit_message>
<xml_diff>
--- a/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
+++ b/LMS_Hackathon/src/test/resources/Test_Data/Team23-TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yours\git\Team23-LMS-Hackathon\LMS_Hackathon\src\test\resources\Test_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanj\git\Team23-LMS-Hackathon\LMS_Hackathon\src\test\resources\Test_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8ADC43A-10E9-466D-86FE-C9E9BBA5E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11938496-9997-4D27-8346-59EA55239707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="65">
   <si>
     <t>username</t>
   </si>
@@ -46,12 +46,6 @@
     <t>programDescription</t>
   </si>
   <si>
-    <t>Team23JavaS</t>
-  </si>
-  <si>
-    <t>AutomationTeam23cod</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -212,6 +206,18 @@
   </si>
   <si>
     <t>ghe@gmail.com</t>
+  </si>
+  <si>
+    <t>Team23JavaSDET</t>
+  </si>
+  <si>
+    <t>AutomationCoding</t>
+  </si>
+  <si>
+    <t>Team23JavaProgram</t>
+  </si>
+  <si>
+    <t>AutomationJavaCode</t>
   </si>
 </sst>
 </file>
@@ -287,15 +293,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -558,15 +562,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A0BF687-F25D-4899-BC43-1B7EA74765DC}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" customWidth="1"/>
     <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -580,10 +584,20 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -595,240 +609,224 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F22F8EA-D627-4EC3-9A1D-2EB34ED5611E}">
   <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <sheetData>
     <row r="1" spans="1:14">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="F1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="G1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="K1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="L1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="M1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="N1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="7" t="s">
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="7" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="E2" s="1">
+        <v>5678905432</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="H2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="7">
-        <v>5678905432</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="F3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="7"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="J3" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="8" t="s">
+      <c r="K3" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="7" t="s">
+      <c r="L3" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M3" s="7" t="s">
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N3" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4" s="7" t="s">
+      <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="D4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="E4" s="1">
+        <v>78654</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="J4" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="7">
-        <v>78654</v>
-      </c>
-      <c r="F4" s="8" t="s">
+      <c r="K4" s="1">
+        <v>123</v>
+      </c>
+      <c r="L4" s="1">
+        <v>345</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="7" t="s">
+      <c r="N4" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="K4" s="7">
-        <v>123</v>
-      </c>
-      <c r="L4" s="7">
-        <v>345</v>
-      </c>
-      <c r="M4" s="7" t="s">
+      <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5" s="7" t="s">
+      <c r="C5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="E5" s="1">
+        <v>3452678910</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="7" t="s">
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="7">
-        <v>3452678910</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="K5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="L5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5" s="7" t="s">
+      <c r="N5" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3456789045</v>
+      </c>
+      <c r="F6" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="G6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L5" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E6" s="7">
-        <v>3456789045</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="M6" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" s="7" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -854,30 +852,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="13.5">
       <c r="A1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>

</xml_diff>